<commit_message>
data added / Minor UI issues fixed / Codes Modified / Responsive issue fixed | Two data files need to be added
</commit_message>
<xml_diff>
--- a/public/data/arz_mabar.xlsx
+++ b/public/data/arz_mabar.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Hominex\mahallat\public\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8640B1E-FBA2-4024-8D99-9BAA8D8B20C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -28,8 +34,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -92,13 +98,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -136,7 +150,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -170,6 +184,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -204,9 +219,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -379,14 +395,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="17.5546875" customWidth="1"/>
+    <col min="2" max="2" width="20.21875" customWidth="1"/>
+    <col min="3" max="3" width="29.44140625" customWidth="1"/>
+    <col min="4" max="4" width="32.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -397,7 +419,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>6</v>
       </c>
@@ -405,10 +427,10 @@
         <v>13</v>
       </c>
       <c r="C2">
-        <v>579.6844395924566</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+        <v>579.68443959245656</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>8</v>
       </c>
@@ -416,10 +438,10 @@
         <v>15</v>
       </c>
       <c r="C3">
-        <v>1766.679827730755</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
+        <v>1766.6798277307551</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>10</v>
       </c>
@@ -427,10 +449,10 @@
         <v>3</v>
       </c>
       <c r="C4">
-        <v>499.0562554445021</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
+        <v>499.05625544450209</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>12</v>
       </c>
@@ -438,10 +460,10 @@
         <v>1</v>
       </c>
       <c r="C5">
-        <v>167.9347465759628</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
+        <v>167.93474657596281</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>16</v>
       </c>
@@ -452,7 +474,7 @@
         <v>191.7284332513762</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>18</v>
       </c>
@@ -460,10 +482,10 @@
         <v>1</v>
       </c>
       <c r="C7">
-        <v>548.3330981045024</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
+        <v>548.33309810450237</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>20</v>
       </c>
@@ -471,10 +493,10 @@
         <v>2</v>
       </c>
       <c r="C8">
-        <v>648.2239236016025</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
+        <v>648.22392360160245</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>24</v>
       </c>
@@ -482,10 +504,10 @@
         <v>2</v>
       </c>
       <c r="C9">
-        <v>380.2918240353912</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
+        <v>380.29182403539119</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>30</v>
       </c>

</xml_diff>